<commit_message>
presentation done, pending aesthetics
</commit_message>
<xml_diff>
--- a/reporte_estadistico/data/gas/metricsCategorias/metrics_21/cat5/metrics_data_tcon.xlsx
+++ b/reporte_estadistico/data/gas/metricsCategorias/metrics_21/cat5/metrics_data_tcon.xlsx
@@ -1,21 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\JJ\repos\research_eslatina\reporte_estadistico\data\gas\metricsCategorias\metrics_21\cat5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quant0</t>
+  </si>
+  <si>
+    <t>quant25</t>
+  </si>
+  <si>
+    <t>quant50</t>
+  </si>
+  <si>
+    <t>quant75</t>
+  </si>
+  <si>
+    <t>quant100</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std_dev</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Estrato1_tcon</t>
+  </si>
+  <si>
+    <t>Estrato2_tcon</t>
+  </si>
+  <si>
+    <t>Estrato3_tcon</t>
+  </si>
+  <si>
+    <t>Estrato4_tcon</t>
+  </si>
+  <si>
+    <t>Estrato5_tcon</t>
+  </si>
+  <si>
+    <t>Estrato6_tcon</t>
+  </si>
+  <si>
+    <t>totResidencial_tcon</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +130,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +216,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,234 +427,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quant0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>quant25</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>quant50</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>quant75</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>quant100</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>skewness</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kurtosis</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>std_dev</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>variance</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Estrato1_tcon</t>
-        </is>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>9550</v>
       </c>
       <c r="C2">
-        <v>2843.25</v>
+        <v>386536.5</v>
       </c>
       <c r="D2">
-        <v>8228</v>
+        <v>755998</v>
       </c>
       <c r="E2">
-        <v>20751.5</v>
+        <v>1796655.5</v>
       </c>
       <c r="F2">
-        <v>126023</v>
+        <v>36788535</v>
       </c>
       <c r="G2">
-        <v>1.079924121213283</v>
+        <v>1.5450586842373619</v>
       </c>
       <c r="H2">
-        <v>3.311172493433669</v>
+        <v>4.6356190747911503</v>
       </c>
       <c r="I2">
-        <v>8228</v>
+        <v>755998</v>
       </c>
       <c r="J2">
-        <v>24869.33848446532</v>
+        <v>4174139.4670978389</v>
       </c>
       <c r="K2">
-        <v>618483996.6549079</v>
+        <v>17423440290783.83</v>
       </c>
       <c r="L2">
-        <v>17847.25</v>
+        <v>2039672.9205298009</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Estrato2_tcon</t>
-        </is>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>57166</v>
       </c>
       <c r="C3">
-        <v>5144</v>
+        <v>684601</v>
       </c>
       <c r="D3">
-        <v>25903</v>
+        <v>1103137</v>
       </c>
       <c r="E3">
-        <v>49654.25</v>
+        <v>2606334.5</v>
       </c>
       <c r="F3">
-        <v>94044</v>
+        <v>141716714</v>
       </c>
       <c r="G3">
-        <v>0.2452625710170625</v>
+        <v>1.4746093098578199</v>
       </c>
       <c r="H3">
-        <v>1.835909080126652</v>
+        <v>4.6569079309710126</v>
       </c>
       <c r="I3">
-        <v>25903</v>
+        <v>1103137</v>
       </c>
       <c r="J3">
-        <v>25723.36073738092</v>
+        <v>12013232.12449014</v>
       </c>
       <c r="K3">
-        <v>661691287.6254302</v>
+        <v>144317746076882</v>
       </c>
       <c r="L3">
-        <v>30527.01829268293</v>
+        <v>3418668.6423841058</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estrato3_tcon</t>
-        </is>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>159874</v>
       </c>
       <c r="D4">
-        <v>70.5</v>
+        <v>410423</v>
       </c>
       <c r="E4">
-        <v>1907.75</v>
+        <v>1716230.5</v>
       </c>
       <c r="F4">
-        <v>47083</v>
+        <v>116240840</v>
       </c>
       <c r="G4">
-        <v>2.415759011944417</v>
+        <v>1.546121847259375</v>
       </c>
       <c r="H4">
-        <v>8.934140147082347</v>
+        <v>4.3574274531185573</v>
       </c>
       <c r="I4">
-        <v>70.5</v>
+        <v>410423</v>
       </c>
       <c r="J4">
-        <v>7627.011212723954</v>
+        <v>9887154.8198739458</v>
       </c>
       <c r="K4">
-        <v>58171300.03901691</v>
+        <v>97755830432156.609</v>
       </c>
       <c r="L4">
-        <v>3112.701219512195</v>
+        <v>2333596.1192052979</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Estrato4_tcon</t>
-        </is>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2988</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>46834</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>575477.5</v>
       </c>
       <c r="F5">
-        <v>19629</v>
+        <v>52406010</v>
+      </c>
+      <c r="G5">
+        <v>1.8402987066699601</v>
+      </c>
+      <c r="H5">
+        <v>5.3582695665439601</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>46834</v>
       </c>
       <c r="J5">
-        <v>1900.169574591332</v>
+        <v>4448314.8393078102</v>
       </c>
       <c r="K5">
-        <v>3610644.412202604</v>
+        <v>19787504909606.07</v>
       </c>
       <c r="L5">
-        <v>266.1524390243902</v>
+        <v>914468.81456953648</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Estrato5_tcon</t>
-        </is>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -586,32 +637,36 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>48423.5</v>
       </c>
       <c r="F6">
-        <v>54</v>
+        <v>21432497</v>
+      </c>
+      <c r="G6">
+        <v>3.1147243016460768</v>
+      </c>
+      <c r="H6">
+        <v>12.127726432884071</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="J6">
-        <v>4.216691570992364</v>
+        <v>1981159.00810098</v>
       </c>
       <c r="K6">
-        <v>17.78048780487805</v>
+        <v>3924991015379.6611</v>
       </c>
       <c r="L6">
-        <v>0.3292682926829268</v>
+        <v>391067.67549668881</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Estrato6_tcon</t>
-        </is>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -623,62 +678,66 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>3480.5</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>24680294</v>
+      </c>
+      <c r="G7">
+        <v>3.970560252411496</v>
+      </c>
+      <c r="H7">
+        <v>18.567912906161499</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2171974.8133110618</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>4717474589657.624</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>358336.70198675501</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>totResidencial_tcon</t>
-        </is>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>538094</v>
       </c>
       <c r="C8">
-        <v>25470.75</v>
+        <v>1484744</v>
       </c>
       <c r="D8">
-        <v>52107.5</v>
+        <v>2762085</v>
       </c>
       <c r="E8">
-        <v>78140.25</v>
+        <v>6653858.5</v>
       </c>
       <c r="F8">
-        <v>150641</v>
+        <v>393264890</v>
       </c>
       <c r="G8">
-        <v>-0.1656855157267</v>
+        <v>1.7486533935934181</v>
       </c>
       <c r="H8">
-        <v>1.800995286038714</v>
+        <v>5.6020651368529926</v>
       </c>
       <c r="I8">
-        <v>52107.5</v>
+        <v>2762085</v>
       </c>
       <c r="J8">
-        <v>33884.80815693017</v>
+        <v>33726588.52851139</v>
       </c>
       <c r="K8">
-        <v>1148180223.831962</v>
+        <v>1137482773771516</v>
       </c>
       <c r="L8">
-        <v>51753.45121951219</v>
+        <v>9455810.8741721846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>